<commit_message>
Return reference positions in SAM/FASTA converter.
</commit_message>
<xml_diff>
--- a/tests/data/SAMtoFASTA.xlsx
+++ b/tests/data/SAMtoFASTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenshank/Documents/Haplotypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C820FD-B493-C64F-B2B8-ACAD353891CA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9078778-1EBB-F74A-84DA-EB6BDE142490}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="6200" windowWidth="35320" windowHeight="18240" xr2:uid="{1120CFA8-2F9C-A643-9C72-DCB3095AFF2C}"/>
+    <workbookView xWindow="9940" yWindow="660" windowWidth="38320" windowHeight="18120" xr2:uid="{1120CFA8-2F9C-A643-9C72-DCB3095AFF2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="65">
   <si>
     <t>Window start</t>
   </si>
@@ -733,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD63090-4388-CE43-8DF4-EA2A839F43C0}">
-  <dimension ref="A1:AB23"/>
+  <dimension ref="A1:AC23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,9 +748,10 @@
     <col min="26" max="26" width="13.83203125" customWidth="1"/>
     <col min="27" max="27" width="12.6640625" customWidth="1"/>
     <col min="28" max="28" width="15.1640625" customWidth="1"/>
+    <col min="29" max="29" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,7 +818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -842,8 +843,8 @@
       <c r="H2" s="3">
         <v>5</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>27</v>
+      <c r="I2" s="3">
+        <v>5</v>
       </c>
       <c r="J2" s="3">
         <v>6</v>
@@ -866,11 +867,11 @@
       <c r="P2" s="3">
         <v>12</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>27</v>
+      <c r="Q2" s="3">
+        <v>12</v>
+      </c>
+      <c r="R2" s="3">
+        <v>12</v>
       </c>
       <c r="S2" s="3">
         <v>13</v>
@@ -894,7 +895,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -976,8 +977,9 @@
       <c r="AB3" s="4" t="s">
         <v>33</v>
       </c>
+      <c r="AC3" s="4"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="4" t="s">
         <v>3</v>
@@ -1061,7 +1063,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
@@ -1227,7 +1229,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
@@ -1310,7 +1312,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -1394,7 +1396,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1560,7 +1562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
@@ -1644,7 +1646,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>11</v>
       </c>
@@ -1727,7 +1729,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
         <v>13</v>
@@ -1894,7 +1896,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
@@ -1977,7 +1979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Adds ability to get FASTA within a window from SAM.
</commit_message>
<xml_diff>
--- a/tests/data/SAMtoFASTA.xlsx
+++ b/tests/data/SAMtoFASTA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenshank/Documents/Haplotypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9078778-1EBB-F74A-84DA-EB6BDE142490}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D9DA22-A81A-9A45-9B7E-371D8DC34505}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9940" yWindow="660" windowWidth="38320" windowHeight="18120" xr2:uid="{1120CFA8-2F9C-A643-9C72-DCB3095AFF2C}"/>
+    <workbookView xWindow="11520" yWindow="5320" windowWidth="38320" windowHeight="18120" xr2:uid="{1120CFA8-2F9C-A643-9C72-DCB3095AFF2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,9 +204,6 @@
     <t>9M1I5M</t>
   </si>
   <si>
-    <t>8M1D3M</t>
-  </si>
-  <si>
     <t>3M1D9M</t>
   </si>
   <si>
@@ -220,6 +217,9 @@
   </si>
   <si>
     <t>~</t>
+  </si>
+  <si>
+    <t>8M1D4M</t>
   </si>
 </sst>
 </file>
@@ -736,7 +736,7 @@
   <dimension ref="A1:AC23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="169" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,7 +892,7 @@
         <v>18</v>
       </c>
       <c r="Y2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -1027,28 +1027,28 @@
         <v>25</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U4" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y4" t="s">
         <v>37</v>
@@ -1068,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
@@ -1119,19 +1119,19 @@
         <v>24</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y5" t="s">
         <v>38</v>
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="AA5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB5" t="s">
         <v>34</v>
@@ -1151,7 +1151,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
@@ -1202,19 +1202,19 @@
         <v>25</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U6" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y6" t="s">
         <v>41</v>
@@ -1234,7 +1234,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
@@ -1285,19 +1285,19 @@
         <v>25</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="U7" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y7" t="s">
         <v>42</v>
@@ -1318,10 +1318,10 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="14" t="s">
         <v>25</v>
@@ -1372,16 +1372,16 @@
         <v>24</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X8" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y8" t="s">
         <v>43</v>
@@ -1401,10 +1401,10 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>25</v>
@@ -1455,19 +1455,19 @@
         <v>24</v>
       </c>
       <c r="U9" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z9">
         <v>2</v>
@@ -1484,10 +1484,10 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>25</v>
@@ -1541,13 +1541,13 @@
         <v>23</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y10" t="s">
         <v>44</v>
@@ -1568,10 +1568,10 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>25</v>
@@ -1625,13 +1625,13 @@
         <v>23</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X11" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y11" t="s">
         <v>45</v>
@@ -1651,10 +1651,10 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>25</v>
@@ -1708,13 +1708,13 @@
         <v>23</v>
       </c>
       <c r="V12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y12" t="s">
         <v>40</v>
@@ -1734,13 +1734,13 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>25</v>
@@ -1791,13 +1791,13 @@
         <v>23</v>
       </c>
       <c r="V13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X13" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y13" t="s">
         <v>46</v>
@@ -1818,13 +1818,13 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>25</v>
@@ -1875,13 +1875,13 @@
         <v>23</v>
       </c>
       <c r="V14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X14" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y14" t="s">
         <v>36</v>
@@ -1893,7 +1893,7 @@
         <v>16</v>
       </c>
       <c r="AB14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -1901,13 +1901,13 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>25</v>
@@ -1961,10 +1961,10 @@
         <v>23</v>
       </c>
       <c r="W15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X15" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y15" t="s">
         <v>47</v>
@@ -1984,13 +1984,13 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>25</v>
@@ -2044,10 +2044,10 @@
         <v>23</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="X16" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y16" t="s">
         <v>48</v>
@@ -2068,16 +2068,16 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>26</v>
@@ -2131,7 +2131,7 @@
         <v>25</v>
       </c>
       <c r="X17" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y17" t="s">
         <v>49</v>
@@ -2151,16 +2151,16 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>26</v>
@@ -2214,7 +2214,7 @@
         <v>25</v>
       </c>
       <c r="X18" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y18" t="s">
         <v>50</v>
@@ -2234,19 +2234,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>23</v>
@@ -2297,7 +2297,7 @@
         <v>25</v>
       </c>
       <c r="X19" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y19" t="s">
         <v>51</v>
@@ -2309,7 +2309,7 @@
         <v>18</v>
       </c>
       <c r="AB19" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
@@ -2317,19 +2317,19 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>23</v>
@@ -2400,25 +2400,25 @@
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>25</v>
@@ -2483,25 +2483,25 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>25</v>
@@ -2566,25 +2566,25 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J23" s="8" t="s">
         <v>25</v>
@@ -2641,7 +2641,7 @@
         <v>19</v>
       </c>
       <c r="AB23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>